<commit_message>
Working on removing sculkwood
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\MC Modding\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E671821E-5DBB-447B-BA0D-503310D4AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C6585-436F-439E-88C5-96650B26F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,18 +81,12 @@
     <t>Warden Chasing</t>
   </si>
   <si>
-    <t>The Faceless</t>
-  </si>
-  <si>
     <t>Plays when the Warden first spawns and begins searching for the player. The Warden is a powerful amalgamation of soul energies and sculk, and its only weaknesses are its blindness and its chest.</t>
   </si>
   <si>
     <t>Plays when the Warden chases the player. The Warden is an indomitable force of death and must be escaped at all costs.</t>
   </si>
   <si>
-    <t>Plays when the Faceless fights the player. The Faceless often haunts players even as they only begin to become insane, but at low sanity levels, it finally confronts the player.</t>
-  </si>
-  <si>
     <t>The Lord's Phantasm</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>This dimension is the afterlife. It was tainted by the affliction when the ancients' lust for eternal life condemned them. It is also where Elrunez resides.</t>
+  </si>
+  <si>
+    <t>The Mirthless</t>
+  </si>
+  <si>
+    <t>Plays when the Mirthless fights the player. The Mirthless often haunts players even as they only begin to become insane, but at low sanity levels, it finally confronts the player.</t>
   </si>
 </sst>
 </file>
@@ -281,10 +281,10 @@
   <autoFilter ref="A1:E19" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{44F286B8-39E0-4372-9A35-DD9C96243317}" name="Track" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{BA1F16DB-2CC9-44EF-94CB-EB1AB6A67C09}" name="Major Motifs" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E9EA6A4B-2A33-4EFE-8731-2A46DBE068DB}" name="Moderate Motifs" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0FFEA9D9-CF62-4F9D-BB65-1EF2F32FF522}" name="Minor Motifs" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{BA1F16DB-2CC9-44EF-94CB-EB1AB6A67C09}" name="Major Motifs" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{E9EA6A4B-2A33-4EFE-8731-2A46DBE068DB}" name="Moderate Motifs" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{0FFEA9D9-CF62-4F9D-BB65-1EF2F32FF522}" name="Minor Motifs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -556,7 +556,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +620,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -633,7 +633,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -643,10 +643,10 @@
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -681,30 +681,30 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -716,10 +716,10 @@
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -742,13 +742,13 @@
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
@@ -757,23 +757,23 @@
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -783,57 +783,57 @@
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Moved hellsteel effects to trinkets
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\MC Modding\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36C6585-436F-439E-88C5-96650B26F47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6FEEA0-5058-41EA-AE90-E9C2562536A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,10 +168,10 @@
     <t>This dimension is the afterlife. It was tainted by the affliction when the ancients' lust for eternal life condemned them. It is also where Elrunez resides.</t>
   </si>
   <si>
-    <t>The Mirthless</t>
-  </si>
-  <si>
-    <t>Plays when the Mirthless fights the player. The Mirthless often haunts players even as they only begin to become insane, but at low sanity levels, it finally confronts the player.</t>
+    <t>The Acharos</t>
+  </si>
+  <si>
+    <t>Plays when the Acharos fights the player. The Acharos often haunts players even as they only begin to become insane, but at low sanity levels, it finally confronts the player.</t>
   </si>
 </sst>
 </file>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Strife now creates pillars on mob hits
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\Modding MC\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F2834F-3A28-436A-8D44-C8FB84C4E56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E600E23-EE44-474F-BD05-4B0CD235DC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Track</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Insanity</t>
   </si>
   <si>
-    <t>Plays when the player has low sanity and is attacked by tormentors. Might also play when the player encounters a non-hostile Faceless.</t>
-  </si>
-  <si>
     <t>Elrunez</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Affliction, Anguish</t>
   </si>
   <si>
-    <t>Affliction's Heart</t>
-  </si>
-  <si>
     <t>Important Motifs</t>
   </si>
   <si>
@@ -174,14 +168,26 @@
     <t>This is Elrunez's final form if the player manages to assemble the Atlas of Frosyni.</t>
   </si>
   <si>
-    <t>It's finally come to it. A battle with Elrunez, the Lord of Torment, creator of the player. He created the player as a vessel that could create and wield the Atlas of Frosyni, but he seems to have failed. Or so it seems.</t>
+    <t>Affliction's Image</t>
+  </si>
+  <si>
+    <t>This is Elrunez's second form.</t>
+  </si>
+  <si>
+    <t>Lord of Torment</t>
+  </si>
+  <si>
+    <t>It's finally come to it. A battle with Elrunez, the Divine Ruler, the Lord of Torment, and the creator of the player. He created the player as a vessel that could create and wield the Atlas of Frosyni, but he seems to have failed. Or so it seems.</t>
+  </si>
+  <si>
+    <t>Plays when the player has low sanity and is attacked by tormentors. Might also play when the player encounters a non-hostile Acharos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +199,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,13 +242,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -280,8 +297,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:E19" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:E19" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:E20" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{44F286B8-39E0-4372-9A35-DD9C96243317}" name="Track" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="3"/>
@@ -556,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,13 +597,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
@@ -609,22 +626,22 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -634,10 +651,10 @@
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -647,68 +664,68 @@
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
+      <c r="A9" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -720,10 +737,10 @@
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -733,10 +750,10 @@
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -746,38 +763,38 @@
     </row>
     <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -785,61 +802,76 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cosmic Egg & Placeholder Track
Added placeholder track for Dread Moon, though it does not play. Note that placeholder tracks with the lead stripped will be used until I can ensure my copyright on the actual tracks.
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\Modding MC\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E600E23-EE44-474F-BD05-4B0CD235DC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064615C2-5F2D-4F41-842E-E867DFEB0E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>Track</t>
   </si>
@@ -102,9 +102,6 @@
     <t>When the player manages to activate the Ancient Portal, corrupted spirits of those who once inhabited the city rise from the ground as energy surges from the portal. This marks the Architect's Siege.</t>
   </si>
   <si>
-    <t>Wraith King</t>
-  </si>
-  <si>
     <t>The boss of the Architect's Siege, spawning after enough waves of mobs have been cleared. It is a conglomeration of spirits that roughly resembles the Warden, and it must be slain to make the portal useable.</t>
   </si>
   <si>
@@ -181,13 +178,31 @@
   </si>
   <si>
     <t>Plays when the player has low sanity and is attacked by tormentors. Might also play when the player encounters a non-hostile Acharos.</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Fallen Sentinel</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>The Demons of the Past</t>
+  </si>
+  <si>
+    <t>Dreams of the Future</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,21 +218,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -242,14 +273,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -257,7 +305,10 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -297,14 +348,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="6" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:E20" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{44F286B8-39E0-4372-9A35-DD9C96243317}" name="Track" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{BA1F16DB-2CC9-44EF-94CB-EB1AB6A67C09}" name="Important Motifs" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E9EA6A4B-2A33-4EFE-8731-2A46DBE068DB}" name="Moderate Motifs" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{0FFEA9D9-CF62-4F9D-BB65-1EF2F32FF522}" name="Acknowledged Motifs" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:F20" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F20" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{44F286B8-39E0-4372-9A35-DD9C96243317}" name="Track" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BA1F16DB-2CC9-44EF-94CB-EB1AB6A67C09}" name="Important Motifs" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E9EA6A4B-2A33-4EFE-8731-2A46DBE068DB}" name="Moderate Motifs" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0FFEA9D9-CF62-4F9D-BB65-1EF2F32FF522}" name="Acknowledged Motifs" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F324D180-2C48-490B-8FC2-ADD1A2924471}" name="Key" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -573,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,9 +639,10 @@
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="28.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,17 +650,20 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -620,13 +676,16 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -635,9 +694,15 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -648,9 +713,15 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -661,24 +732,30 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -689,9 +766,10 @@
         <v>7</v>
       </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -704,9 +782,10 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -719,13 +798,16 @@
       <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -734,9 +816,12 @@
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -747,26 +832,30 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>18</v>
@@ -775,54 +864,66 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>22</v>
@@ -831,13 +932,16 @@
       <c r="E17" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>47</v>
+      <c r="F17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>22</v>
@@ -846,33 +950,38 @@
       <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Gilded Marble Block
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\Modding MC\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064615C2-5F2D-4F41-842E-E867DFEB0E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F92BC0-4C86-4A6D-9037-BE4B55B6C326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Track</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Anguish, Holy</t>
   </si>
   <si>
-    <t>Elrunez, Affliction</t>
-  </si>
-  <si>
     <t>Architect's Siege</t>
   </si>
   <si>
@@ -196,6 +193,21 @@
   </si>
   <si>
     <t>Dreams of the Future</t>
+  </si>
+  <si>
+    <t>Ender Dragon Approach</t>
+  </si>
+  <si>
+    <t>Plays as the player approaches the sleeping Ender Dragon.</t>
+  </si>
+  <si>
+    <t>Finale</t>
+  </si>
+  <si>
+    <t>Elrunez, Finale</t>
+  </si>
+  <si>
+    <t>Elrunez, Affliction, Finale</t>
   </si>
 </sst>
 </file>
@@ -273,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -292,12 +304,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -348,8 +354,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:F20" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F20" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}" name="Table3" displayName="Table3" ref="A1:F21" totalsRowShown="0" dataDxfId="6" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F21" xr:uid="{99D8C478-FF24-485C-A27D-740352D838C9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{44F286B8-39E0-4372-9A35-DD9C96243317}" name="Track" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{16734576-B6DD-4BED-933E-7FCEC034B1F2}" name="Description" dataDxfId="4"/>
@@ -625,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,20 +656,20 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -677,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -685,7 +691,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
@@ -695,10 +701,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -714,10 +720,10 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -733,255 +739,269 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="F14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>52</v>
+      <c r="F21" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redid the end gold source
</commit_message>
<xml_diff>
--- a/src/main/resources/Music Tracks.xlsx
+++ b/src/main/resources/Music Tracks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsta\Documents\Modding MC\dndreams\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF933C81-CB4A-4F3E-B688-DCC202ECF374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1EA7E9-9464-44FF-9695-13739EB9DDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="5040" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>Major</t>
   </si>
   <si>
-    <t>The Demons of the Past</t>
-  </si>
-  <si>
     <t>Dreams of the Future</t>
   </si>
   <si>
@@ -214,13 +211,16 @@
   </si>
   <si>
     <t>Major -&gt; Minor</t>
+  </si>
+  <si>
+    <t>Demons of the Past</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +232,14 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -310,6 +318,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -639,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,14 +704,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -712,7 +723,7 @@
         <v>51</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -731,7 +742,7 @@
         <v>51</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -770,13 +781,13 @@
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -805,7 +816,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
@@ -954,7 +965,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
@@ -972,7 +983,7 @@
         <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
@@ -1009,7 +1020,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>